<commit_message>
Start refactoring the basestation
</commit_message>
<xml_diff>
--- a/weather_station_settings.xlsx
+++ b/weather_station_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Benjamin\Documents\git\weatherstation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A124313-2733-494B-B725-8F0EC5773801}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F36764B0-542E-45E8-A0D7-D7D21FB14ECA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{FF36C336-DBE7-42B9-A89D-5D5EC9FFE05A}"/>
   </bookViews>
@@ -468,7 +468,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="4"/>
@@ -487,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="6" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Accent3" xfId="6" builtinId="40"/>
@@ -502,13 +503,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -517,6 +511,13 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -546,9 +547,9 @@
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{208D5548-998D-4DCD-8CF3-83EDF216FB51}">
       <tableStyleElement type="wholeTable" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
-      <tableStyleElement type="firstColumnStripe" size="4" dxfId="2"/>
-      <tableStyleElement type="secondColumnStripe" size="4" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="firstColumnStripe" size="4" dxfId="1"/>
+      <tableStyleElement type="secondColumnStripe" size="4" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -869,7 +870,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M12" sqref="M12"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1837,7 @@
       <c r="U4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="V4" s="18" t="s">
         <v>58</v>
       </c>
       <c r="W4" s="9">
@@ -1849,7 +1850,7 @@
       <c r="Y4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Z4" s="17" t="s">
         <v>59</v>
       </c>
       <c r="AA4" s="8">
@@ -1922,7 +1923,7 @@
         <v>67</v>
       </c>
       <c r="K5" s="11">
-        <f>G5+H5</f>
+        <f t="shared" ref="K5:K30" si="11">G5+H5</f>
         <v>2</v>
       </c>
       <c r="L5" s="11">
@@ -1935,7 +1936,7 @@
         <v>69</v>
       </c>
       <c r="O5" s="12">
-        <f>K5+L5</f>
+        <f t="shared" ref="O5:O30" si="12">K5+L5</f>
         <v>6</v>
       </c>
       <c r="P5" s="12"/>
@@ -2024,15 +2025,15 @@
         <v>0</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" ref="G6:G30" si="11">C6+D6</f>
+        <f t="shared" ref="G6:G30" si="13">C6+D6</f>
         <v>0</v>
       </c>
       <c r="K6" s="8">
-        <f>G6+H6</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O6" s="9">
-        <f>K6+L6</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S6" s="8">
@@ -2090,21 +2091,21 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="11">
-        <f>G7+H7</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="12">
-        <f>K7+L7</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P7" s="12"/>
@@ -2193,15 +2194,15 @@
         <v>0</v>
       </c>
       <c r="G8" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K8" s="8">
-        <f>G8+H8</f>
-        <v>0</v>
-      </c>
       <c r="O8" s="9">
-        <f>K8+L8</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S8" s="8">
@@ -2259,21 +2260,21 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="11">
-        <f>G9+H9</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="12">
-        <f>K9+L9</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P9" s="12"/>
@@ -2362,15 +2363,15 @@
         <v>0</v>
       </c>
       <c r="G10" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K10" s="8">
-        <f>G10+H10</f>
-        <v>0</v>
-      </c>
       <c r="O10" s="9">
-        <f>K10+L10</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S10" s="8">
@@ -2428,21 +2429,21 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="11">
-        <f>G11+H11</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="12">
-        <f>K11+L11</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P11" s="12"/>
@@ -2531,15 +2532,15 @@
         <v>0</v>
       </c>
       <c r="G12" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K12" s="8">
-        <f>G12+H12</f>
-        <v>0</v>
-      </c>
       <c r="O12" s="9">
-        <f>K12+L12</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S12" s="8">
@@ -2597,21 +2598,21 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="11">
-        <f>G13+H13</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="12">
-        <f>K13+L13</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P13" s="12"/>
@@ -2700,15 +2701,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K14" s="8">
-        <f>G14+H14</f>
-        <v>0</v>
-      </c>
       <c r="O14" s="9">
-        <f>K14+L14</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S14" s="8">
@@ -2766,21 +2767,21 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="11">
-        <f>G15+H15</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="12">
-        <f>K15+L15</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P15" s="12"/>
@@ -2869,15 +2870,15 @@
         <v>0</v>
       </c>
       <c r="G16" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K16" s="8">
-        <f>G16+H16</f>
-        <v>0</v>
-      </c>
       <c r="O16" s="9">
-        <f>K16+L16</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S16" s="8">
@@ -2935,21 +2936,21 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="11">
-        <f>G17+H17</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="12">
-        <f>K17+L17</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P17" s="12"/>
@@ -3038,15 +3039,15 @@
         <v>0</v>
       </c>
       <c r="G18" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K18" s="8">
-        <f>G18+H18</f>
-        <v>0</v>
-      </c>
       <c r="O18" s="9">
-        <f>K18+L18</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S18" s="8">
@@ -3104,21 +3105,21 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="11">
-        <f>G19+H19</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="12">
-        <f>K19+L19</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P19" s="12"/>
@@ -3207,15 +3208,15 @@
         <v>0</v>
       </c>
       <c r="G20" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K20" s="8">
-        <f>G20+H20</f>
-        <v>0</v>
-      </c>
       <c r="O20" s="9">
-        <f>K20+L20</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S20" s="8">
@@ -3273,21 +3274,21 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="11">
-        <f>G21+H21</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="12">
-        <f>K21+L21</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P21" s="12"/>
@@ -3376,15 +3377,15 @@
         <v>0</v>
       </c>
       <c r="G22" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K22" s="8">
-        <f>G22+H22</f>
-        <v>0</v>
-      </c>
       <c r="O22" s="9">
-        <f>K22+L22</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S22" s="8">
@@ -3442,21 +3443,21 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="11">
-        <f>G23+H23</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="12">
-        <f>K23+L23</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P23" s="12"/>
@@ -3545,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K24" s="8">
-        <f>G24+H24</f>
-        <v>0</v>
-      </c>
       <c r="O24" s="9">
-        <f>K24+L24</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S24" s="8">
@@ -3611,21 +3612,21 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="11">
-        <f>G25+H25</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="12">
-        <f>K25+L25</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P25" s="12"/>
@@ -3714,15 +3715,15 @@
         <v>0</v>
       </c>
       <c r="G26" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K26" s="8">
-        <f>G26+H26</f>
-        <v>0</v>
-      </c>
       <c r="O26" s="9">
-        <f>K26+L26</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S26" s="8">
@@ -3780,21 +3781,21 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="11">
-        <f>G27+H27</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="12">
-        <f>K27+L27</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P27" s="12"/>
@@ -3883,15 +3884,15 @@
         <v>0</v>
       </c>
       <c r="G28" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K28" s="8">
-        <f>G28+H28</f>
-        <v>0</v>
-      </c>
       <c r="O28" s="9">
-        <f>K28+L28</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S28" s="8">
@@ -3949,21 +3950,21 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="11">
-        <f>G29+H29</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="12">
-        <f>K29+L29</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P29" s="12"/>
@@ -4052,15 +4053,15 @@
         <v>0</v>
       </c>
       <c r="G30" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K30" s="8">
-        <f>G30+H30</f>
-        <v>0</v>
-      </c>
       <c r="O30" s="9">
-        <f>K30+L30</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S30" s="8">

</xml_diff>